<commit_message>
free bonus - redeem code - loyalty server...
</commit_message>
<xml_diff>
--- a/features/backlog/android/SignUp_SymlexVPN.xlsx
+++ b/features/backlog/android/SignUp_SymlexVPN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97346544-CC11-4557-9C0A-E6B15F118386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E18560-070E-4CC3-8A6A-A4C5DD631E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="540" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="signup" sheetId="1" r:id="rId1"/>
@@ -1490,7 +1490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>